<commit_message>
Added new data stream pages, still a bit rough
</commit_message>
<xml_diff>
--- a/app/src/main/res/DummyData.xlsx
+++ b/app/src/main/res/DummyData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Philip\Documents\GitHub\125project\app\src\main\res\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E22E961D-DD91-480A-A599-0B0C769273A6}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BFD8CA8-C247-439C-B476-7A55F8C6A5F3}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{99F8E762-9D4E-476B-A086-3E63E408ECA1}"/>
   </bookViews>
@@ -550,47 +550,47 @@
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2">
         <f ca="1">INT(RAND()*10000)</f>
-        <v>7771</v>
+        <v>8540</v>
       </c>
       <c r="B2">
         <f t="shared" ref="B2:G2" ca="1" si="0">INT(RAND()*10000)</f>
-        <v>8859</v>
+        <v>276</v>
       </c>
       <c r="C2">
         <f t="shared" ca="1" si="0"/>
-        <v>6074</v>
+        <v>6624</v>
       </c>
       <c r="D2">
         <f t="shared" ca="1" si="0"/>
-        <v>5091</v>
+        <v>5708</v>
       </c>
       <c r="E2">
         <f t="shared" ca="1" si="0"/>
-        <v>46</v>
+        <v>8008</v>
       </c>
       <c r="F2">
         <f t="shared" ca="1" si="0"/>
-        <v>9723</v>
+        <v>6918</v>
       </c>
       <c r="G2">
         <f t="shared" ca="1" si="0"/>
-        <v>7369</v>
+        <v>9378</v>
       </c>
       <c r="H2">
         <f ca="1">INT(SUM(A2:G2)/7)</f>
-        <v>6419</v>
+        <v>6493</v>
       </c>
       <c r="I2">
         <f ca="1">INT(STDEV(A2:G2))</f>
-        <v>3217</v>
+        <v>3007</v>
       </c>
       <c r="J2">
         <f ca="1">H2 - 1.5 * I2</f>
-        <v>1593.5</v>
+        <v>1982.5</v>
       </c>
       <c r="K2">
         <f ca="1">H2 + 1.5 * I2</f>
-        <v>11244.5</v>
+        <v>11003.5</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
@@ -704,35 +704,35 @@
       </c>
       <c r="B2">
         <f ca="1" xml:space="preserve"> INT(RAND()*100 +40)</f>
-        <v>105</v>
+        <v>135</v>
       </c>
       <c r="C2">
         <f t="shared" ref="C2:H17" ca="1" si="0" xml:space="preserve"> INT(RAND()*100 +40)</f>
-        <v>111</v>
+        <v>77</v>
       </c>
       <c r="D2">
         <f t="shared" ca="1" si="0"/>
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="E2">
         <f t="shared" ca="1" si="0"/>
-        <v>59</v>
+        <v>86</v>
       </c>
       <c r="F2">
         <f t="shared" ca="1" si="0"/>
-        <v>67</v>
+        <v>101</v>
       </c>
       <c r="G2">
         <f t="shared" ca="1" si="0"/>
-        <v>77</v>
+        <v>63</v>
       </c>
       <c r="H2">
         <f t="shared" ca="1" si="0"/>
-        <v>86</v>
+        <v>132</v>
       </c>
       <c r="I2">
         <f ca="1">INT(AVERAGE(B2:H2))</f>
-        <v>90</v>
+        <v>103</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -741,35 +741,35 @@
       </c>
       <c r="B3">
         <f t="shared" ref="B3:H25" ca="1" si="1" xml:space="preserve"> INT(RAND()*100 +40)</f>
+        <v>48</v>
+      </c>
+      <c r="C3">
+        <f t="shared" ca="1" si="0"/>
+        <v>47</v>
+      </c>
+      <c r="D3">
+        <f t="shared" ca="1" si="0"/>
+        <v>118</v>
+      </c>
+      <c r="E3">
+        <f t="shared" ca="1" si="0"/>
+        <v>88</v>
+      </c>
+      <c r="F3">
+        <f t="shared" ca="1" si="0"/>
+        <v>134</v>
+      </c>
+      <c r="G3">
+        <f t="shared" ca="1" si="0"/>
         <v>93</v>
       </c>
-      <c r="C3">
-        <f t="shared" ca="1" si="0"/>
-        <v>98</v>
-      </c>
-      <c r="D3">
-        <f t="shared" ca="1" si="0"/>
-        <v>97</v>
-      </c>
-      <c r="E3">
-        <f t="shared" ca="1" si="0"/>
-        <v>115</v>
-      </c>
-      <c r="F3">
-        <f t="shared" ca="1" si="0"/>
-        <v>80</v>
-      </c>
-      <c r="G3">
-        <f t="shared" ca="1" si="0"/>
-        <v>78</v>
-      </c>
       <c r="H3">
         <f t="shared" ca="1" si="0"/>
-        <v>93</v>
+        <v>110</v>
       </c>
       <c r="I3">
         <f t="shared" ref="I3:I25" ca="1" si="2">INT(AVERAGE(B3:H3))</f>
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -778,35 +778,35 @@
       </c>
       <c r="B4">
         <f t="shared" ca="1" si="1"/>
-        <v>129</v>
+        <v>48</v>
       </c>
       <c r="C4">
         <f t="shared" ca="1" si="0"/>
-        <v>68</v>
+        <v>126</v>
       </c>
       <c r="D4">
         <f t="shared" ca="1" si="0"/>
-        <v>57</v>
+        <v>102</v>
       </c>
       <c r="E4">
         <f t="shared" ca="1" si="0"/>
-        <v>98</v>
+        <v>87</v>
       </c>
       <c r="F4">
         <f t="shared" ca="1" si="0"/>
-        <v>66</v>
+        <v>94</v>
       </c>
       <c r="G4">
         <f t="shared" ca="1" si="0"/>
-        <v>139</v>
+        <v>51</v>
       </c>
       <c r="H4">
         <f t="shared" ca="1" si="0"/>
-        <v>94</v>
+        <v>135</v>
       </c>
       <c r="I4">
         <f t="shared" ca="1" si="2"/>
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -815,35 +815,35 @@
       </c>
       <c r="B5">
         <f t="shared" ca="1" si="1"/>
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="C5">
         <f t="shared" ca="1" si="0"/>
-        <v>126</v>
+        <v>117</v>
       </c>
       <c r="D5">
         <f t="shared" ca="1" si="0"/>
-        <v>104</v>
+        <v>42</v>
       </c>
       <c r="E5">
         <f t="shared" ca="1" si="0"/>
-        <v>103</v>
+        <v>113</v>
       </c>
       <c r="F5">
         <f t="shared" ca="1" si="0"/>
-        <v>106</v>
+        <v>133</v>
       </c>
       <c r="G5">
         <f t="shared" ca="1" si="0"/>
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="H5">
         <f t="shared" ca="1" si="0"/>
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="I5">
         <f t="shared" ca="1" si="2"/>
-        <v>104</v>
+        <v>97</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -852,35 +852,35 @@
       </c>
       <c r="B6">
         <f t="shared" ca="1" si="1"/>
-        <v>50</v>
+        <v>122</v>
       </c>
       <c r="C6">
         <f t="shared" ca="1" si="0"/>
-        <v>44</v>
+        <v>83</v>
       </c>
       <c r="D6">
         <f t="shared" ca="1" si="0"/>
-        <v>135</v>
+        <v>126</v>
       </c>
       <c r="E6">
         <f t="shared" ca="1" si="0"/>
-        <v>49</v>
+        <v>88</v>
       </c>
       <c r="F6">
         <f t="shared" ca="1" si="0"/>
+        <v>58</v>
+      </c>
+      <c r="G6">
+        <f t="shared" ca="1" si="0"/>
+        <v>101</v>
+      </c>
+      <c r="H6">
+        <f t="shared" ca="1" si="0"/>
         <v>97</v>
       </c>
-      <c r="G6">
-        <f t="shared" ca="1" si="0"/>
-        <v>80</v>
-      </c>
-      <c r="H6">
-        <f t="shared" ca="1" si="0"/>
-        <v>42</v>
-      </c>
       <c r="I6">
         <f t="shared" ca="1" si="2"/>
-        <v>71</v>
+        <v>96</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
@@ -889,35 +889,35 @@
       </c>
       <c r="B7">
         <f t="shared" ca="1" si="1"/>
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C7">
         <f t="shared" ca="1" si="0"/>
-        <v>40</v>
+        <v>63</v>
       </c>
       <c r="D7">
         <f t="shared" ca="1" si="0"/>
-        <v>126</v>
+        <v>48</v>
       </c>
       <c r="E7">
         <f t="shared" ca="1" si="0"/>
-        <v>120</v>
+        <v>57</v>
       </c>
       <c r="F7">
         <f t="shared" ca="1" si="0"/>
-        <v>68</v>
+        <v>111</v>
       </c>
       <c r="G7">
         <f t="shared" ca="1" si="0"/>
-        <v>86</v>
+        <v>60</v>
       </c>
       <c r="H7">
         <f t="shared" ca="1" si="0"/>
-        <v>115</v>
+        <v>128</v>
       </c>
       <c r="I7">
         <f t="shared" ca="1" si="2"/>
-        <v>86</v>
+        <v>74</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
@@ -926,35 +926,35 @@
       </c>
       <c r="B8">
         <f t="shared" ca="1" si="1"/>
-        <v>111</v>
+        <v>128</v>
       </c>
       <c r="C8">
         <f t="shared" ca="1" si="0"/>
-        <v>44</v>
+        <v>67</v>
       </c>
       <c r="D8">
         <f t="shared" ca="1" si="0"/>
+        <v>51</v>
+      </c>
+      <c r="E8">
+        <f t="shared" ca="1" si="0"/>
+        <v>74</v>
+      </c>
+      <c r="F8">
+        <f t="shared" ca="1" si="0"/>
+        <v>56</v>
+      </c>
+      <c r="G8">
+        <f t="shared" ca="1" si="0"/>
+        <v>49</v>
+      </c>
+      <c r="H8">
+        <f t="shared" ca="1" si="0"/>
+        <v>123</v>
+      </c>
+      <c r="I8">
+        <f t="shared" ca="1" si="2"/>
         <v>78</v>
-      </c>
-      <c r="E8">
-        <f t="shared" ca="1" si="0"/>
-        <v>99</v>
-      </c>
-      <c r="F8">
-        <f t="shared" ca="1" si="0"/>
-        <v>63</v>
-      </c>
-      <c r="G8">
-        <f t="shared" ca="1" si="0"/>
-        <v>78</v>
-      </c>
-      <c r="H8">
-        <f t="shared" ca="1" si="0"/>
-        <v>48</v>
-      </c>
-      <c r="I8">
-        <f t="shared" ca="1" si="2"/>
-        <v>74</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
@@ -963,15 +963,15 @@
       </c>
       <c r="B9">
         <f t="shared" ca="1" si="1"/>
-        <v>109</v>
+        <v>139</v>
       </c>
       <c r="C9">
         <f t="shared" ca="1" si="0"/>
-        <v>91</v>
+        <v>113</v>
       </c>
       <c r="D9">
         <f t="shared" ca="1" si="0"/>
-        <v>93</v>
+        <v>115</v>
       </c>
       <c r="E9">
         <f t="shared" ca="1" si="0"/>
@@ -979,19 +979,19 @@
       </c>
       <c r="F9">
         <f t="shared" ca="1" si="0"/>
-        <v>96</v>
+        <v>53</v>
       </c>
       <c r="G9">
         <f t="shared" ca="1" si="0"/>
-        <v>50</v>
+        <v>112</v>
       </c>
       <c r="H9">
         <f t="shared" ca="1" si="0"/>
-        <v>88</v>
+        <v>138</v>
       </c>
       <c r="I9">
         <f t="shared" ca="1" si="2"/>
-        <v>81</v>
+        <v>101</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
@@ -1000,35 +1000,35 @@
       </c>
       <c r="B10">
         <f t="shared" ca="1" si="1"/>
-        <v>88</v>
+        <v>127</v>
       </c>
       <c r="C10">
         <f t="shared" ca="1" si="0"/>
-        <v>89</v>
+        <v>133</v>
       </c>
       <c r="D10">
         <f t="shared" ca="1" si="0"/>
-        <v>112</v>
+        <v>43</v>
       </c>
       <c r="E10">
         <f t="shared" ca="1" si="0"/>
+        <v>96</v>
+      </c>
+      <c r="F10">
+        <f t="shared" ca="1" si="0"/>
+        <v>139</v>
+      </c>
+      <c r="G10">
+        <f t="shared" ca="1" si="0"/>
+        <v>49</v>
+      </c>
+      <c r="H10">
+        <f t="shared" ca="1" si="0"/>
         <v>120</v>
       </c>
-      <c r="F10">
-        <f t="shared" ca="1" si="0"/>
-        <v>52</v>
-      </c>
-      <c r="G10">
-        <f t="shared" ca="1" si="0"/>
-        <v>63</v>
-      </c>
-      <c r="H10">
-        <f t="shared" ca="1" si="0"/>
-        <v>83</v>
-      </c>
       <c r="I10">
         <f t="shared" ca="1" si="2"/>
-        <v>86</v>
+        <v>101</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
@@ -1037,35 +1037,35 @@
       </c>
       <c r="B11">
         <f t="shared" ca="1" si="1"/>
-        <v>107</v>
+        <v>115</v>
       </c>
       <c r="C11">
         <f t="shared" ca="1" si="0"/>
+        <v>113</v>
+      </c>
+      <c r="D11">
+        <f t="shared" ca="1" si="0"/>
         <v>43</v>
       </c>
-      <c r="D11">
+      <c r="E11">
+        <f t="shared" ca="1" si="0"/>
+        <v>98</v>
+      </c>
+      <c r="F11">
         <f t="shared" ca="1" si="0"/>
         <v>112</v>
       </c>
-      <c r="E11">
-        <f t="shared" ca="1" si="0"/>
-        <v>101</v>
-      </c>
-      <c r="F11">
-        <f t="shared" ca="1" si="0"/>
-        <v>99</v>
-      </c>
       <c r="G11">
         <f t="shared" ca="1" si="0"/>
-        <v>71</v>
+        <v>41</v>
       </c>
       <c r="H11">
         <f t="shared" ca="1" si="0"/>
-        <v>107</v>
+        <v>92</v>
       </c>
       <c r="I11">
         <f t="shared" ca="1" si="2"/>
-        <v>91</v>
+        <v>87</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
@@ -1074,35 +1074,35 @@
       </c>
       <c r="B12">
         <f t="shared" ca="1" si="1"/>
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="C12">
         <f t="shared" ca="1" si="0"/>
-        <v>129</v>
+        <v>60</v>
       </c>
       <c r="D12">
         <f t="shared" ca="1" si="0"/>
-        <v>106</v>
+        <v>62</v>
       </c>
       <c r="E12">
         <f t="shared" ca="1" si="0"/>
-        <v>47</v>
+        <v>124</v>
       </c>
       <c r="F12">
         <f t="shared" ca="1" si="0"/>
-        <v>129</v>
+        <v>109</v>
       </c>
       <c r="G12">
         <f t="shared" ca="1" si="0"/>
-        <v>128</v>
+        <v>75</v>
       </c>
       <c r="H12">
         <f t="shared" ca="1" si="0"/>
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="I12">
         <f t="shared" ca="1" si="2"/>
-        <v>104</v>
+        <v>87</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
@@ -1111,35 +1111,35 @@
       </c>
       <c r="B13">
         <f t="shared" ca="1" si="1"/>
-        <v>54</v>
+        <v>118</v>
       </c>
       <c r="C13">
         <f t="shared" ca="1" si="0"/>
-        <v>48</v>
+        <v>62</v>
       </c>
       <c r="D13">
         <f t="shared" ca="1" si="0"/>
-        <v>120</v>
+        <v>88</v>
       </c>
       <c r="E13">
         <f t="shared" ca="1" si="0"/>
-        <v>66</v>
+        <v>80</v>
       </c>
       <c r="F13">
         <f t="shared" ca="1" si="0"/>
-        <v>58</v>
+        <v>132</v>
       </c>
       <c r="G13">
         <f t="shared" ca="1" si="0"/>
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="H13">
         <f t="shared" ca="1" si="0"/>
-        <v>68</v>
+        <v>137</v>
       </c>
       <c r="I13">
         <f t="shared" ca="1" si="2"/>
-        <v>70</v>
+        <v>99</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
@@ -1148,35 +1148,35 @@
       </c>
       <c r="B14">
         <f t="shared" ca="1" si="1"/>
-        <v>121</v>
+        <v>50</v>
       </c>
       <c r="C14">
         <f t="shared" ca="1" si="0"/>
+        <v>97</v>
+      </c>
+      <c r="D14">
+        <f t="shared" ca="1" si="0"/>
+        <v>64</v>
+      </c>
+      <c r="E14">
+        <f t="shared" ca="1" si="0"/>
+        <v>75</v>
+      </c>
+      <c r="F14">
+        <f t="shared" ca="1" si="0"/>
+        <v>125</v>
+      </c>
+      <c r="G14">
+        <f t="shared" ca="1" si="0"/>
+        <v>120</v>
+      </c>
+      <c r="H14">
+        <f t="shared" ca="1" si="0"/>
         <v>41</v>
       </c>
-      <c r="D14">
-        <f t="shared" ca="1" si="0"/>
-        <v>59</v>
-      </c>
-      <c r="E14">
-        <f t="shared" ca="1" si="0"/>
-        <v>102</v>
-      </c>
-      <c r="F14">
-        <f t="shared" ca="1" si="0"/>
-        <v>89</v>
-      </c>
-      <c r="G14">
-        <f t="shared" ca="1" si="0"/>
-        <v>102</v>
-      </c>
-      <c r="H14">
-        <f t="shared" ca="1" si="0"/>
-        <v>126</v>
-      </c>
       <c r="I14">
         <f t="shared" ca="1" si="2"/>
-        <v>91</v>
+        <v>81</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
@@ -1185,35 +1185,35 @@
       </c>
       <c r="B15">
         <f t="shared" ca="1" si="1"/>
-        <v>78</v>
+        <v>47</v>
       </c>
       <c r="C15">
         <f t="shared" ca="1" si="0"/>
-        <v>79</v>
+        <v>62</v>
       </c>
       <c r="D15">
         <f t="shared" ca="1" si="0"/>
-        <v>70</v>
+        <v>125</v>
       </c>
       <c r="E15">
         <f t="shared" ca="1" si="0"/>
-        <v>44</v>
+        <v>138</v>
       </c>
       <c r="F15">
         <f t="shared" ca="1" si="0"/>
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="G15">
         <f t="shared" ca="1" si="0"/>
-        <v>87</v>
+        <v>117</v>
       </c>
       <c r="H15">
         <f t="shared" ca="1" si="0"/>
-        <v>48</v>
+        <v>71</v>
       </c>
       <c r="I15">
         <f t="shared" ca="1" si="2"/>
-        <v>76</v>
+        <v>97</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
@@ -1222,35 +1222,35 @@
       </c>
       <c r="B16">
         <f t="shared" ca="1" si="1"/>
-        <v>111</v>
+        <v>95</v>
       </c>
       <c r="C16">
         <f t="shared" ca="1" si="0"/>
-        <v>82</v>
+        <v>97</v>
       </c>
       <c r="D16">
         <f t="shared" ca="1" si="0"/>
-        <v>78</v>
+        <v>44</v>
       </c>
       <c r="E16">
         <f t="shared" ca="1" si="0"/>
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="F16">
         <f t="shared" ca="1" si="0"/>
-        <v>109</v>
+        <v>129</v>
       </c>
       <c r="G16">
         <f t="shared" ca="1" si="0"/>
-        <v>56</v>
+        <v>117</v>
       </c>
       <c r="H16">
         <f t="shared" ca="1" si="0"/>
-        <v>121</v>
+        <v>66</v>
       </c>
       <c r="I16">
         <f t="shared" ca="1" si="2"/>
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="K16" t="s">
         <v>16</v>
@@ -1262,35 +1262,35 @@
       </c>
       <c r="B17">
         <f t="shared" ca="1" si="1"/>
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="C17">
         <f t="shared" ca="1" si="0"/>
-        <v>110</v>
+        <v>58</v>
       </c>
       <c r="D17">
         <f t="shared" ca="1" si="0"/>
-        <v>109</v>
+        <v>79</v>
       </c>
       <c r="E17">
         <f t="shared" ca="1" si="0"/>
-        <v>88</v>
+        <v>50</v>
       </c>
       <c r="F17">
         <f t="shared" ca="1" si="0"/>
-        <v>89</v>
+        <v>136</v>
       </c>
       <c r="G17">
         <f t="shared" ca="1" si="0"/>
-        <v>119</v>
+        <v>97</v>
       </c>
       <c r="H17">
         <f t="shared" ca="1" si="0"/>
-        <v>85</v>
+        <v>47</v>
       </c>
       <c r="I17">
         <f t="shared" ca="1" si="2"/>
-        <v>95</v>
+        <v>78</v>
       </c>
       <c r="K17" t="s">
         <v>16</v>
@@ -1302,35 +1302,35 @@
       </c>
       <c r="B18">
         <f t="shared" ca="1" si="1"/>
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="C18">
         <f t="shared" ca="1" si="1"/>
-        <v>87</v>
+        <v>139</v>
       </c>
       <c r="D18">
         <f t="shared" ca="1" si="1"/>
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E18">
         <f t="shared" ca="1" si="1"/>
-        <v>55</v>
+        <v>91</v>
       </c>
       <c r="F18">
         <f t="shared" ca="1" si="1"/>
-        <v>43</v>
+        <v>83</v>
       </c>
       <c r="G18">
         <f t="shared" ca="1" si="1"/>
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="H18">
         <f t="shared" ca="1" si="1"/>
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="I18">
         <f t="shared" ca="1" si="2"/>
-        <v>69</v>
+        <v>86</v>
       </c>
       <c r="K18" t="s">
         <v>15</v>
@@ -1342,35 +1342,35 @@
       </c>
       <c r="B19">
         <f t="shared" ca="1" si="1"/>
-        <v>126</v>
+        <v>89</v>
       </c>
       <c r="C19">
         <f t="shared" ca="1" si="1"/>
+        <v>79</v>
+      </c>
+      <c r="D19">
+        <f t="shared" ca="1" si="1"/>
+        <v>82</v>
+      </c>
+      <c r="E19">
+        <f t="shared" ca="1" si="1"/>
+        <v>87</v>
+      </c>
+      <c r="F19">
+        <f t="shared" ca="1" si="1"/>
+        <v>40</v>
+      </c>
+      <c r="G19">
+        <f t="shared" ca="1" si="1"/>
+        <v>86</v>
+      </c>
+      <c r="H19">
+        <f t="shared" ca="1" si="1"/>
         <v>73</v>
       </c>
-      <c r="D19">
-        <f t="shared" ca="1" si="1"/>
-        <v>79</v>
-      </c>
-      <c r="E19">
-        <f t="shared" ca="1" si="1"/>
-        <v>65</v>
-      </c>
-      <c r="F19">
-        <f t="shared" ca="1" si="1"/>
-        <v>84</v>
-      </c>
-      <c r="G19">
-        <f t="shared" ca="1" si="1"/>
-        <v>71</v>
-      </c>
-      <c r="H19">
-        <f t="shared" ca="1" si="1"/>
-        <v>103</v>
-      </c>
       <c r="I19">
         <f t="shared" ca="1" si="2"/>
-        <v>85</v>
+        <v>76</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
@@ -1379,35 +1379,35 @@
       </c>
       <c r="B20">
         <f t="shared" ca="1" si="1"/>
-        <v>47</v>
+        <v>63</v>
       </c>
       <c r="C20">
         <f t="shared" ca="1" si="1"/>
-        <v>135</v>
+        <v>40</v>
       </c>
       <c r="D20">
         <f t="shared" ca="1" si="1"/>
-        <v>134</v>
+        <v>117</v>
       </c>
       <c r="E20">
         <f t="shared" ca="1" si="1"/>
-        <v>81</v>
+        <v>66</v>
       </c>
       <c r="F20">
         <f t="shared" ca="1" si="1"/>
+        <v>51</v>
+      </c>
+      <c r="G20">
+        <f t="shared" ca="1" si="1"/>
         <v>97</v>
       </c>
-      <c r="G20">
-        <f t="shared" ca="1" si="1"/>
-        <v>106</v>
-      </c>
       <c r="H20">
         <f t="shared" ca="1" si="1"/>
-        <v>64</v>
+        <v>101</v>
       </c>
       <c r="I20">
         <f t="shared" ca="1" si="2"/>
-        <v>94</v>
+        <v>76</v>
       </c>
       <c r="K20" t="s">
         <v>11</v>
@@ -1419,35 +1419,35 @@
       </c>
       <c r="B21">
         <f t="shared" ca="1" si="1"/>
+        <v>53</v>
+      </c>
+      <c r="C21">
+        <f t="shared" ca="1" si="1"/>
         <v>79</v>
       </c>
-      <c r="C21">
-        <f t="shared" ca="1" si="1"/>
-        <v>41</v>
-      </c>
       <c r="D21">
         <f t="shared" ca="1" si="1"/>
-        <v>70</v>
+        <v>79</v>
       </c>
       <c r="E21">
         <f t="shared" ca="1" si="1"/>
-        <v>84</v>
+        <v>94</v>
       </c>
       <c r="F21">
         <f t="shared" ca="1" si="1"/>
-        <v>85</v>
+        <v>124</v>
       </c>
       <c r="G21">
         <f t="shared" ca="1" si="1"/>
+        <v>44</v>
+      </c>
+      <c r="H21">
+        <f t="shared" ca="1" si="1"/>
         <v>48</v>
       </c>
-      <c r="H21">
-        <f t="shared" ca="1" si="1"/>
-        <v>68</v>
-      </c>
       <c r="I21">
         <f t="shared" ca="1" si="2"/>
-        <v>67</v>
+        <v>74</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
@@ -1456,35 +1456,35 @@
       </c>
       <c r="B22">
         <f t="shared" ca="1" si="1"/>
-        <v>97</v>
+        <v>54</v>
       </c>
       <c r="C22">
         <f t="shared" ca="1" si="1"/>
-        <v>118</v>
+        <v>83</v>
       </c>
       <c r="D22">
         <f t="shared" ca="1" si="1"/>
-        <v>90</v>
+        <v>70</v>
       </c>
       <c r="E22">
         <f t="shared" ca="1" si="1"/>
-        <v>139</v>
+        <v>69</v>
       </c>
       <c r="F22">
         <f t="shared" ca="1" si="1"/>
-        <v>46</v>
+        <v>82</v>
       </c>
       <c r="G22">
         <f t="shared" ca="1" si="1"/>
-        <v>52</v>
+        <v>73</v>
       </c>
       <c r="H22">
         <f t="shared" ca="1" si="1"/>
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="I22">
         <f t="shared" ca="1" si="2"/>
-        <v>94</v>
+        <v>77</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
@@ -1493,35 +1493,35 @@
       </c>
       <c r="B23">
         <f t="shared" ca="1" si="1"/>
-        <v>40</v>
+        <v>138</v>
       </c>
       <c r="C23">
         <f t="shared" ca="1" si="1"/>
-        <v>124</v>
+        <v>94</v>
       </c>
       <c r="D23">
         <f t="shared" ca="1" si="1"/>
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="E23">
         <f t="shared" ca="1" si="1"/>
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="F23">
         <f t="shared" ca="1" si="1"/>
-        <v>122</v>
+        <v>131</v>
       </c>
       <c r="G23">
         <f t="shared" ca="1" si="1"/>
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="H23">
         <f t="shared" ca="1" si="1"/>
-        <v>122</v>
+        <v>54</v>
       </c>
       <c r="I23">
         <f t="shared" ca="1" si="2"/>
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="K23" t="s">
         <v>13</v>
@@ -1533,35 +1533,35 @@
       </c>
       <c r="B24">
         <f t="shared" ca="1" si="1"/>
-        <v>122</v>
+        <v>78</v>
       </c>
       <c r="C24">
         <f t="shared" ca="1" si="1"/>
-        <v>72</v>
+        <v>58</v>
       </c>
       <c r="D24">
         <f t="shared" ca="1" si="1"/>
-        <v>86</v>
+        <v>109</v>
       </c>
       <c r="E24">
         <f t="shared" ca="1" si="1"/>
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F24">
         <f t="shared" ca="1" si="1"/>
-        <v>103</v>
+        <v>46</v>
       </c>
       <c r="G24">
         <f t="shared" ca="1" si="1"/>
+        <v>40</v>
+      </c>
+      <c r="H24">
+        <f t="shared" ca="1" si="1"/>
         <v>139</v>
       </c>
-      <c r="H24">
-        <f t="shared" ca="1" si="1"/>
-        <v>106</v>
-      </c>
       <c r="I24">
         <f t="shared" ca="1" si="2"/>
-        <v>96</v>
+        <v>73</v>
       </c>
       <c r="K24" t="s">
         <v>12</v>
@@ -1573,35 +1573,35 @@
       </c>
       <c r="B25">
         <f t="shared" ca="1" si="1"/>
-        <v>40</v>
+        <v>71</v>
       </c>
       <c r="C25">
         <f t="shared" ca="1" si="1"/>
-        <v>64</v>
+        <v>87</v>
       </c>
       <c r="D25">
         <f t="shared" ca="1" si="1"/>
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="E25">
         <f t="shared" ca="1" si="1"/>
-        <v>113</v>
+        <v>68</v>
       </c>
       <c r="F25">
         <f t="shared" ca="1" si="1"/>
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="G25">
         <f t="shared" ca="1" si="1"/>
-        <v>53</v>
+        <v>107</v>
       </c>
       <c r="H25">
         <f t="shared" ca="1" si="1"/>
-        <v>114</v>
+        <v>120</v>
       </c>
       <c r="I25">
         <f t="shared" ca="1" si="2"/>
-        <v>68</v>
+        <v>78</v>
       </c>
       <c r="K25" t="s">
         <v>11</v>
@@ -1613,32 +1613,32 @@
         <v>86</v>
       </c>
       <c r="C26">
-        <f t="shared" ref="C26:I26" ca="1" si="3">INT(AVERAGE(C2:C25))</f>
-        <v>81</v>
+        <f t="shared" ref="C26:H26" ca="1" si="3">INT(AVERAGE(C2:C25))</f>
+        <v>84</v>
       </c>
       <c r="D26">
         <f t="shared" ca="1" si="3"/>
-        <v>92</v>
+        <v>79</v>
       </c>
       <c r="E26">
         <f t="shared" ca="1" si="3"/>
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F26">
         <f t="shared" ca="1" si="3"/>
-        <v>84</v>
+        <v>98</v>
       </c>
       <c r="G26">
         <f t="shared" ca="1" si="3"/>
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="H26">
         <f t="shared" ca="1" si="3"/>
-        <v>88</v>
+        <v>95</v>
       </c>
       <c r="I26">
         <f ca="1">INT(AVERAGE(I2:I25))</f>
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
   </sheetData>

</xml_diff>